<commit_message>
Better bragg and interferometer
</commit_message>
<xml_diff>
--- a/mwav_f23 alex and torda/bragg/lattice constant calculations.xlsx
+++ b/mwav_f23 alex and torda/bragg/lattice constant calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stlgo\Documents\Github\phy417s-mw\mwav_f23 alex and torda\bragg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB98B13-8D27-4554-982E-3BD169D095D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA835D5-1278-4ABD-94F6-48A300A30A2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="1515" windowWidth="21600" windowHeight="11295" xr2:uid="{8AF79E62-D719-4D4C-8DA7-221C583B9319}"/>
+    <workbookView xWindow="-615" yWindow="1995" windowWidth="17175" windowHeight="11295" xr2:uid="{8AF79E62-D719-4D4C-8DA7-221C583B9319}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -426,7 +426,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,10 +445,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2.6840000000000002</v>
+        <v>2.82</v>
       </c>
       <c r="B2">
-        <v>0.54</v>
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -479,29 +479,29 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>18</v>
+        <v>17.61</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>1.9</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5">
         <f>$A$2/(2*(SIN(B5*3.14/180)))</f>
-        <v>4.3449330296568762</v>
+        <v>4.6628875677088049</v>
       </c>
       <c r="F5">
         <f>E5*SQRT(($B$2/$A$2)^2 +(SIN(C5*PI()/180)/SIN(B5*PI()/180))^2)</f>
-        <v>1.3138331410173569</v>
+        <v>0.51281463829277674</v>
       </c>
       <c r="G5">
         <f>E5/D5</f>
-        <v>4.3449330296568762</v>
+        <v>4.6628875677088049</v>
       </c>
       <c r="H5">
         <f>F5/D5</f>
-        <v>1.3138331410173569</v>
+        <v>0.51281463829277674</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -509,10 +509,10 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>27</v>
+        <v>27.82</v>
       </c>
       <c r="C6">
-        <v>2.5</v>
+        <v>2.9</v>
       </c>
       <c r="D6">
         <f>SQRT(2)</f>
@@ -520,19 +520,19 @@
       </c>
       <c r="E6">
         <f>D6*$A$2/(2*(SIN(B6*PI()/180)))</f>
-        <v>4.1804280085012788</v>
+        <v>4.2726822896568226</v>
       </c>
       <c r="F6">
         <f t="shared" ref="F6:F7" si="0">E6*SQRT(($B$2/$A$2)^2 +(SIN(C6*PI()/180)/SIN(B6*PI()/180))^2)</f>
-        <v>0.93205433523851422</v>
+        <v>0.46485985606868252</v>
       </c>
       <c r="G6">
         <f t="shared" ref="G6:G7" si="1">E6/D6</f>
-        <v>2.9560089930734281</v>
+        <v>3.0212426208720036</v>
       </c>
       <c r="H6">
         <f t="shared" ref="H6:H7" si="2">F6/D6</f>
-        <v>0.65906194088147307</v>
+        <v>0.32870555652756783</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -540,10 +540,10 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>48</v>
+        <v>48.58</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="D7">
         <f>SQRT(5)</f>
@@ -551,19 +551,19 @@
       </c>
       <c r="E7">
         <f>D7*$A$2/(2*(SIN(B7*3.14/180)))</f>
-        <v>4.0395241482402486</v>
+        <v>4.2060749125484245</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>0.94072209814354291</v>
+        <v>0.48067004979416439</v>
       </c>
       <c r="G7">
         <f t="shared" si="1"/>
-        <v>1.8065301184434266</v>
+        <v>1.881013884582952</v>
       </c>
       <c r="H7">
         <f t="shared" si="2"/>
-        <v>0.42070371187703809</v>
+        <v>0.21496218121759206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>